<commit_message>
Same problem solved in R
</commit_message>
<xml_diff>
--- a/Excel/AirlineRM.xlsx
+++ b/Excel/AirlineRM.xlsx
@@ -648,12 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -667,6 +661,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,50 +1020,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="18"/>
       <c r="B6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="18"/>
       <c r="B7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="18"/>
       <c r="B8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1083,30 +1083,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="22">
         <v>0</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>77408</v>
       </c>
     </row>
@@ -1116,53 +1116,53 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="23">
         <v>0</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="23">
         <v>100</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="22">
         <v>0</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="22">
         <v>66</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1172,82 +1172,82 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="23">
         <v>166</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="23">
         <v>100</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="22">
         <v>66</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="19">
         <v>84</v>
       </c>
     </row>
@@ -1274,17 +1274,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1294,90 +1294,90 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="25" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <v>100</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>0</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="21">
         <v>617</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="21">
         <v>1E+30</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <v>66</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>0</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="19">
         <v>238</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="19">
         <v>379</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="19">
         <v>238</v>
       </c>
     </row>
@@ -1387,113 +1387,113 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="25" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="21">
         <v>166</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="21">
         <v>238</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="21">
         <v>166</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="21">
         <v>84</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="21">
         <v>100</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="21">
         <v>379</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <v>100</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="21">
         <v>66</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="19">
         <v>66</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="19">
         <v>0</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="19">
         <v>150</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="19">
         <v>1E+30</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="19">
         <v>84</v>
       </c>
     </row>
@@ -1521,136 +1521,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="22">
         <v>77408</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="24"/>
+      <c r="F11" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="23">
         <v>100</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="23">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="23">
         <v>15708</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="23">
         <v>100</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="23">
         <v>77408</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="22">
         <v>66</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="22">
         <v>0</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="22">
         <v>61700</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="22">
         <v>66</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="22">
         <v>77408</v>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1723,14 +1723,14 @@
         <v>617</v>
       </c>
       <c r="D5" s="4">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E5" s="5">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>150</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B8" s="7">
         <f>SUMPRODUCT(C5:C6, E5:E6)</f>
-        <v>102422</v>
+        <v>116350</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1791,13 +1791,13 @@
       </c>
       <c r="B11" s="9">
         <f>E5+E6</f>
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="11">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -1807,14 +1807,14 @@
       </c>
       <c r="B12" s="12">
         <f>E5</f>
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="14">
         <f>D5</f>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="B13" s="12">
         <f>E6</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>19</v>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B14" s="12">
         <f>E5</f>
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>20</v>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B15" s="15">
         <f>E6</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>20</v>

</xml_diff>